<commit_message>
Ordered translations with separate bulk insert for each language, completed Russian, Armenian and German translations
/* Translation Stats */
SELECT trl_language, COUNT(*) AS translated_strings, 211-COUNT(*) AS ToTranslate
FROM `zzzzsys_translate` GROUP BY trl_language ORDER BY translated_strings DESC, trl_language ASC;
</commit_message>
<xml_diff>
--- a/nub4fixes/docs/NuBuilder Languages.xlsx
+++ b/nub4fixes/docs/NuBuilder Languages.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="1077">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1722" uniqueCount="1080">
   <si>
     <t>trl_english</t>
   </si>
@@ -2899,24 +2899,15 @@
     <t xml:space="preserve">     , COALESCE(b.zzzzsys_translate_id, '') AS zzzzsys_translate_id</t>
   </si>
   <si>
-    <t xml:space="preserve">     , 'Hindi' AS trl_language, a.trl_english</t>
-  </si>
-  <si>
     <t xml:space="preserve">     , COALESCE(b.trl_translation, '') AS trl_translation</t>
   </si>
   <si>
     <t>FROM</t>
   </si>
   <si>
-    <t xml:space="preserve">(SELECT '' AS zzzzsys_translate_id, 'Hindi' AS trl_language, trl_english, '' AS trl_translation FROM `zzzzsys_translate` GROUP BY trl_english) a </t>
-  </si>
-  <si>
     <t xml:space="preserve">LEFT JOIN </t>
   </si>
   <si>
-    <t>(SELECT * FROM zzzzsys_translate WHERE trl_language ='Hindi') b USING (trl_english), (SELECT @a:=0) c</t>
-  </si>
-  <si>
     <t>जब खोज में शामिल करें</t>
   </si>
   <si>
@@ -3251,6 +3242,24 @@
   </si>
   <si>
     <t>nu5bad6cb3aef3155</t>
+  </si>
+  <si>
+    <t>-- Translation Stats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT trl_language, COUNT(*) AS translated_strings, 211-COUNT(*) AS ToTranslate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     , @Lang AS trl_language, a.trl_english</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(SELECT '' AS zzzzsys_translate_id, @Lang AS trl_language, trl_english, '' AS trl_translation FROM `zzzzsys_translate` GROUP BY trl_english) a </t>
+  </si>
+  <si>
+    <t>SET @Lang:='Hindi';</t>
+  </si>
+  <si>
+    <t>FROM `zzzzsys_translate` GROUP BY trl_language ORDER BY translated_strings DESC, trl_language ASC;</t>
   </si>
 </sst>
 </file>
@@ -8120,7 +8129,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="C2" t="s">
         <v>647</v>
@@ -8129,7 +8138,7 @@
         <v>311</v>
       </c>
       <c r="E2" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="F2" t="str">
         <f>"('"&amp;B2&amp;"','"&amp;C2&amp;"','"&amp;D2&amp;"','"&amp;E2&amp;"'),"</f>
@@ -8141,7 +8150,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="C3" t="s">
         <v>647</v>
@@ -8150,7 +8159,7 @@
         <v>312</v>
       </c>
       <c r="E3" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F66" si="0">"('"&amp;B3&amp;"','"&amp;C3&amp;"','"&amp;D3&amp;"','"&amp;E3&amp;"'),"</f>
@@ -8162,7 +8171,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1023</v>
+        <v>1020</v>
       </c>
       <c r="C4" t="s">
         <v>647</v>
@@ -8171,7 +8180,7 @@
         <v>313</v>
       </c>
       <c r="E4" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
@@ -8204,7 +8213,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="C6" t="s">
         <v>647</v>
@@ -8213,7 +8222,7 @@
         <v>314</v>
       </c>
       <c r="E6" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
@@ -8267,7 +8276,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
       <c r="C9" t="s">
         <v>647</v>
@@ -8276,7 +8285,7 @@
         <v>315</v>
       </c>
       <c r="E9" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
@@ -8288,7 +8297,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="C10" t="s">
         <v>647</v>
@@ -8297,7 +8306,7 @@
         <v>316</v>
       </c>
       <c r="E10" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
@@ -8330,7 +8339,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="C12" t="s">
         <v>647</v>
@@ -8339,7 +8348,7 @@
         <v>317</v>
       </c>
       <c r="E12" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
@@ -8771,7 +8780,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="C33" t="s">
         <v>647</v>
@@ -8780,7 +8789,7 @@
         <v>318</v>
       </c>
       <c r="E33" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
@@ -8876,7 +8885,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="C38" t="s">
         <v>647</v>
@@ -8885,7 +8894,7 @@
         <v>319</v>
       </c>
       <c r="E38" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
@@ -8981,7 +8990,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
       <c r="C43" t="s">
         <v>647</v>
@@ -8990,7 +8999,7 @@
         <v>320</v>
       </c>
       <c r="E43" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
@@ -9023,7 +9032,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
       <c r="C45" t="s">
         <v>647</v>
@@ -9032,7 +9041,7 @@
         <v>321</v>
       </c>
       <c r="E45" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
@@ -9128,7 +9137,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="C50" t="s">
         <v>647</v>
@@ -9137,7 +9146,7 @@
         <v>322</v>
       </c>
       <c r="E50" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
       <c r="F50" t="str">
         <f t="shared" si="0"/>
@@ -9149,7 +9158,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="C51" t="s">
         <v>647</v>
@@ -9158,7 +9167,7 @@
         <v>323</v>
       </c>
       <c r="E51" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" si="0"/>
@@ -9170,7 +9179,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="C52" t="s">
         <v>647</v>
@@ -9179,7 +9188,7 @@
         <v>324</v>
       </c>
       <c r="E52" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="F52" t="str">
         <f t="shared" si="0"/>
@@ -9233,7 +9242,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
       <c r="C55" t="s">
         <v>647</v>
@@ -9242,7 +9251,7 @@
         <v>325</v>
       </c>
       <c r="E55" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
       <c r="F55" t="str">
         <f t="shared" si="0"/>
@@ -9254,7 +9263,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="C56" t="s">
         <v>647</v>
@@ -9263,7 +9272,7 @@
         <v>326</v>
       </c>
       <c r="E56" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="F56" t="str">
         <f t="shared" si="0"/>
@@ -9296,7 +9305,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="C58" t="s">
         <v>647</v>
@@ -9305,7 +9314,7 @@
         <v>327</v>
       </c>
       <c r="E58" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="F58" t="str">
         <f t="shared" si="0"/>
@@ -9338,7 +9347,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="C60" t="s">
         <v>647</v>
@@ -9347,7 +9356,7 @@
         <v>328</v>
       </c>
       <c r="E60" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
       <c r="F60" t="str">
         <f t="shared" si="0"/>
@@ -9401,7 +9410,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
       <c r="C63" t="s">
         <v>647</v>
@@ -9410,7 +9419,7 @@
         <v>329</v>
       </c>
       <c r="E63" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
       <c r="F63" t="str">
         <f t="shared" si="0"/>
@@ -9485,7 +9494,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
       <c r="C67" t="s">
         <v>647</v>
@@ -9494,7 +9503,7 @@
         <v>330</v>
       </c>
       <c r="E67" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="F67" t="str">
         <f t="shared" ref="F67:F130" si="1">"('"&amp;B67&amp;"','"&amp;C67&amp;"','"&amp;D67&amp;"','"&amp;E67&amp;"'),"</f>
@@ -9611,7 +9620,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
       <c r="C73" t="s">
         <v>647</v>
@@ -9620,7 +9629,7 @@
         <v>332</v>
       </c>
       <c r="E73" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="F73" t="str">
         <f t="shared" si="1"/>
@@ -9695,7 +9704,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="C77" t="s">
         <v>647</v>
@@ -9704,7 +9713,7 @@
         <v>333</v>
       </c>
       <c r="E77" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
       <c r="F77" t="str">
         <f t="shared" si="1"/>
@@ -9800,7 +9809,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
       <c r="C82" t="s">
         <v>647</v>
@@ -9809,7 +9818,7 @@
         <v>334</v>
       </c>
       <c r="E82" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
       <c r="F82" t="str">
         <f t="shared" si="1"/>
@@ -9821,7 +9830,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
       <c r="C83" t="s">
         <v>647</v>
@@ -9830,7 +9839,7 @@
         <v>335</v>
       </c>
       <c r="E83" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="F83" t="str">
         <f t="shared" si="1"/>
@@ -9884,7 +9893,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
       <c r="C86" t="s">
         <v>647</v>
@@ -9893,7 +9902,7 @@
         <v>336</v>
       </c>
       <c r="E86" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
       <c r="F86" t="str">
         <f t="shared" si="1"/>
@@ -9989,7 +9998,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
       <c r="C91" t="s">
         <v>647</v>
@@ -9998,7 +10007,7 @@
         <v>337</v>
       </c>
       <c r="E91" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
       <c r="F91" t="str">
         <f t="shared" si="1"/>
@@ -10094,7 +10103,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
       <c r="C96" t="s">
         <v>647</v>
@@ -10103,7 +10112,7 @@
         <v>338</v>
       </c>
       <c r="E96" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="F96" t="str">
         <f t="shared" si="1"/>
@@ -10157,7 +10166,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="C99" t="s">
         <v>647</v>
@@ -10166,7 +10175,7 @@
         <v>339</v>
       </c>
       <c r="E99" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
       <c r="F99" t="str">
         <f t="shared" si="1"/>
@@ -10241,7 +10250,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="C103" t="s">
         <v>647</v>
@@ -10250,7 +10259,7 @@
         <v>340</v>
       </c>
       <c r="E103" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="F103" t="str">
         <f t="shared" si="1"/>
@@ -10325,7 +10334,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>1050</v>
+        <v>1047</v>
       </c>
       <c r="C107" t="s">
         <v>647</v>
@@ -10334,7 +10343,7 @@
         <v>341</v>
       </c>
       <c r="E107" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
       <c r="F107" t="str">
         <f t="shared" si="1"/>
@@ -10409,7 +10418,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="C111" t="s">
         <v>647</v>
@@ -10418,7 +10427,7 @@
         <v>342</v>
       </c>
       <c r="E111" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
       <c r="F111" t="str">
         <f t="shared" si="1"/>
@@ -10430,7 +10439,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="C112" t="s">
         <v>647</v>
@@ -10439,7 +10448,7 @@
         <v>343</v>
       </c>
       <c r="E112" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
       <c r="F112" t="str">
         <f t="shared" si="1"/>
@@ -10640,7 +10649,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="C122" t="s">
         <v>647</v>
@@ -10649,7 +10658,7 @@
         <v>344</v>
       </c>
       <c r="E122" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="F122" t="str">
         <f t="shared" si="1"/>
@@ -10661,7 +10670,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="C123" t="s">
         <v>647</v>
@@ -10670,7 +10679,7 @@
         <v>345</v>
       </c>
       <c r="E123" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
       <c r="F123" t="str">
         <f t="shared" si="1"/>
@@ -10682,7 +10691,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="C124" t="s">
         <v>647</v>
@@ -10691,7 +10700,7 @@
         <v>346</v>
       </c>
       <c r="E124" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
       <c r="F124" t="str">
         <f t="shared" si="1"/>
@@ -10766,7 +10775,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="C128" t="s">
         <v>647</v>
@@ -10775,7 +10784,7 @@
         <v>347</v>
       </c>
       <c r="E128" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="F128" t="str">
         <f t="shared" si="1"/>
@@ -10871,7 +10880,7 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
       <c r="C133" t="s">
         <v>647</v>
@@ -10880,7 +10889,7 @@
         <v>838</v>
       </c>
       <c r="E133" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="F133" t="str">
         <f t="shared" si="2"/>
@@ -10913,7 +10922,7 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="C135" t="s">
         <v>647</v>
@@ -10922,7 +10931,7 @@
         <v>349</v>
       </c>
       <c r="E135" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
       <c r="F135" t="str">
         <f t="shared" si="2"/>
@@ -10934,7 +10943,7 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="C136" t="s">
         <v>647</v>
@@ -10943,7 +10952,7 @@
         <v>350</v>
       </c>
       <c r="E136" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
       <c r="F136" t="str">
         <f t="shared" si="2"/>
@@ -11039,7 +11048,7 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
       <c r="C141" t="s">
         <v>647</v>
@@ -11048,7 +11057,7 @@
         <v>351</v>
       </c>
       <c r="E141" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="F141" t="str">
         <f t="shared" si="2"/>
@@ -11060,7 +11069,7 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="C142" t="s">
         <v>647</v>
@@ -11069,7 +11078,7 @@
         <v>352</v>
       </c>
       <c r="E142" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
       <c r="F142" t="str">
         <f t="shared" si="2"/>
@@ -11375,7 +11384,7 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="C157" t="s">
         <v>647</v>
@@ -11384,7 +11393,7 @@
         <v>353</v>
       </c>
       <c r="E157" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="F157" t="str">
         <f t="shared" si="2"/>
@@ -11396,7 +11405,7 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="C158" t="s">
         <v>647</v>
@@ -11405,7 +11414,7 @@
         <v>354</v>
       </c>
       <c r="E158" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="F158" t="str">
         <f t="shared" si="2"/>
@@ -11417,7 +11426,7 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="C159" t="s">
         <v>647</v>
@@ -11426,7 +11435,7 @@
         <v>355</v>
       </c>
       <c r="E159" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="F159" t="str">
         <f t="shared" si="2"/>
@@ -11522,7 +11531,7 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="C164" t="s">
         <v>647</v>
@@ -11531,7 +11540,7 @@
         <v>356</v>
       </c>
       <c r="E164" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="F164" t="str">
         <f t="shared" si="2"/>
@@ -11762,7 +11771,7 @@
         <v>126</v>
       </c>
       <c r="E175" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="F175" t="str">
         <f t="shared" si="2"/>
@@ -11774,7 +11783,7 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="C176" t="s">
         <v>647</v>
@@ -11783,7 +11792,7 @@
         <v>357</v>
       </c>
       <c r="E176" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="F176" t="str">
         <f t="shared" si="2"/>
@@ -11795,7 +11804,7 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="C177" t="s">
         <v>647</v>
@@ -11804,7 +11813,7 @@
         <v>358</v>
       </c>
       <c r="E177" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="F177" t="str">
         <f t="shared" si="2"/>
@@ -11921,7 +11930,7 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
       <c r="C183" t="s">
         <v>647</v>
@@ -11930,7 +11939,7 @@
         <v>155</v>
       </c>
       <c r="E183" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
       <c r="F183" t="str">
         <f t="shared" si="2"/>
@@ -12089,7 +12098,7 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="C191" t="s">
         <v>647</v>
@@ -12098,7 +12107,7 @@
         <v>156</v>
       </c>
       <c r="E191" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
       <c r="F191" t="str">
         <f t="shared" si="2"/>
@@ -12236,7 +12245,7 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="C198" t="s">
         <v>647</v>
@@ -12245,7 +12254,7 @@
         <v>359</v>
       </c>
       <c r="E198" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="F198" t="str">
         <f t="shared" si="3"/>
@@ -12257,7 +12266,7 @@
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>1071</v>
+        <v>1068</v>
       </c>
       <c r="C199" t="s">
         <v>647</v>
@@ -12266,7 +12275,7 @@
         <v>360</v>
       </c>
       <c r="E199" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="F199" t="str">
         <f t="shared" si="3"/>
@@ -12320,7 +12329,7 @@
         <v>201</v>
       </c>
       <c r="B202" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="C202" t="s">
         <v>647</v>
@@ -12329,7 +12338,7 @@
         <v>361</v>
       </c>
       <c r="E202" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
       <c r="F202" t="str">
         <f t="shared" si="3"/>
@@ -12362,7 +12371,7 @@
         <v>203</v>
       </c>
       <c r="B204" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="C204" t="s">
         <v>647</v>
@@ -12371,7 +12380,7 @@
         <v>362</v>
       </c>
       <c r="E204" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="F204" t="str">
         <f t="shared" si="3"/>
@@ -12383,7 +12392,7 @@
         <v>204</v>
       </c>
       <c r="B205" t="s">
-        <v>1074</v>
+        <v>1071</v>
       </c>
       <c r="C205" t="s">
         <v>647</v>
@@ -12392,7 +12401,7 @@
         <v>363</v>
       </c>
       <c r="E205" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="F205" t="str">
         <f t="shared" si="3"/>
@@ -12425,7 +12434,7 @@
         <v>206</v>
       </c>
       <c r="B207" t="s">
-        <v>1075</v>
+        <v>1072</v>
       </c>
       <c r="C207" t="s">
         <v>647</v>
@@ -12434,7 +12443,7 @@
         <v>364</v>
       </c>
       <c r="E207" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="F207" t="str">
         <f t="shared" si="3"/>
@@ -12446,7 +12455,7 @@
         <v>207</v>
       </c>
       <c r="B208" t="s">
-        <v>1076</v>
+        <v>1073</v>
       </c>
       <c r="C208" t="s">
         <v>647</v>
@@ -12455,7 +12464,7 @@
         <v>365</v>
       </c>
       <c r="E208" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="F208" t="str">
         <f t="shared" si="3"/>
@@ -12557,10 +12566,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A28"/>
+  <dimension ref="A1:A33"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12632,42 +12641,60 @@
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="5" t="s">
-        <v>957</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="5" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="5" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="5" t="s">
-        <v>960</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="5" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="5" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="5" t="s">
-        <v>963</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="5" t="s">
-        <v>964</v>
+        <v>961</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="5"/>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="4" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="5" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="5" t="s">
+        <v>1079</v>
       </c>
     </row>
   </sheetData>

</xml_diff>